<commit_message>
Update - 20150531 (2)
</commit_message>
<xml_diff>
--- a/parliament/join_districts.xlsx
+++ b/parliament/join_districts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fousseynou\Google Drive\DS4AFRICA\parliament\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fousseynou\Google Drive\DS4AFRICA\elections\parliament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{651E475D-7C2E-41F6-82A2-7C46F9145A7A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98B8733F-7225-432C-93B0-884FD38B8DDD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{96F22577-583E-452A-9F1D-A8A802497610}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>shapefile</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Bafoulabe</t>
-  </si>
-  <si>
-    <t>Bamako</t>
   </si>
   <si>
     <t>Diema</t>
@@ -603,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0436F098-6DF8-446A-8092-8D4227C05BCC}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +612,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -706,7 +703,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +711,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -722,7 +719,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +727,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,7 +759,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,7 +799,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -834,7 +831,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,7 +871,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,7 +895,7 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,7 +911,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,7 +927,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -946,7 +943,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,7 +991,7 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1018,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1026,7 +1023,7 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1034,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1042,7 +1039,7 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1050,7 +1047,7 @@
         <v>15</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1058,7 +1055,7 @@
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>